<commit_message>
update without male sel offset fishery
</commit_message>
<xml_diff>
--- a/Northern rock sole/Data/2024_ADMB_estimate.xlsx
+++ b/Northern rock sole/Data/2024_ADMB_estimate.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Grant Adams\Documents\GitHub\Rceattle-models\Northern rock sole\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5413B0EC-643D-4DF5-99F3-2AC92BEFC296}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2083BD03-1DDB-4BA9-8EA6-8B0C66F0D5D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="345" yWindow="3150" windowWidth="17610" windowHeight="12420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="2024 SAFE init" sheetId="1" r:id="rId1"/>
+    <sheet name="2024 SAFE" sheetId="1" r:id="rId1"/>
     <sheet name="Recruitment" sheetId="2" r:id="rId2"/>
     <sheet name="SSB" sheetId="3" r:id="rId3"/>
     <sheet name="Total biomass" sheetId="4" r:id="rId4"/>
@@ -419,7 +419,7 @@
   <dimension ref="A1:BA51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -446,16 +446,16 @@
         <v>1975</v>
       </c>
       <c r="B2">
-        <v>290.47300000000001</v>
+        <v>246.19300000000001</v>
       </c>
       <c r="C2">
-        <v>63.967199999999998</v>
+        <v>60.297600000000003</v>
       </c>
       <c r="D2">
-        <v>582.07299999999998</v>
+        <v>485.87299999999999</v>
       </c>
       <c r="E2">
-        <v>12.2552</v>
+        <v>12.239100000000001</v>
       </c>
       <c r="H2" s="1"/>
     </row>
@@ -464,16 +464,16 @@
         <v>1976</v>
       </c>
       <c r="B3">
-        <v>320.43799999999999</v>
+        <v>266.55599999999998</v>
       </c>
       <c r="C3">
-        <v>69.837000000000003</v>
+        <v>63.517699999999998</v>
       </c>
       <c r="D3">
-        <v>1364.42</v>
-      </c>
-      <c r="E3">
-        <v>10.167400000000001</v>
+        <v>1189.76</v>
+      </c>
+      <c r="E3" s="1">
+        <v>10.151199999999999</v>
       </c>
       <c r="H3" s="1"/>
     </row>
@@ -482,16 +482,16 @@
         <v>1977</v>
       </c>
       <c r="B4">
-        <v>343.23099999999999</v>
+        <v>283.40300000000002</v>
       </c>
       <c r="C4">
-        <v>81.614599999999996</v>
+        <v>72.361999999999995</v>
       </c>
       <c r="D4">
-        <v>724.01300000000003</v>
-      </c>
-      <c r="E4" s="1">
-        <v>5.3636299999999997</v>
+        <v>658.94100000000003</v>
+      </c>
+      <c r="E4">
+        <v>5.3811799999999996</v>
       </c>
       <c r="H4" s="1"/>
     </row>
@@ -500,16 +500,16 @@
         <v>1978</v>
       </c>
       <c r="B5">
-        <v>366.041</v>
+        <v>304.36599999999999</v>
       </c>
       <c r="C5">
-        <v>104.245</v>
+        <v>89.991900000000001</v>
       </c>
       <c r="D5">
-        <v>1033.6600000000001</v>
+        <v>959.24</v>
       </c>
       <c r="E5">
-        <v>7.1397000000000004</v>
+        <v>7.1788699999999999</v>
       </c>
       <c r="H5" s="1"/>
     </row>
@@ -518,16 +518,16 @@
         <v>1979</v>
       </c>
       <c r="B6">
-        <v>382.20400000000001</v>
+        <v>322.49299999999999</v>
       </c>
       <c r="C6">
-        <v>127.91200000000001</v>
+        <v>109.605</v>
       </c>
       <c r="D6">
-        <v>947.46100000000001</v>
+        <v>876.851</v>
       </c>
       <c r="E6">
-        <v>5.8743699999999999</v>
+        <v>5.8662900000000002</v>
       </c>
       <c r="H6" s="1"/>
     </row>
@@ -536,16 +536,16 @@
         <v>1980</v>
       </c>
       <c r="B7">
-        <v>405.12599999999998</v>
+        <v>348.09899999999999</v>
       </c>
       <c r="C7">
-        <v>141.31399999999999</v>
+        <v>123.764</v>
       </c>
       <c r="D7">
-        <v>1206.3399999999999</v>
+        <v>1111.1099999999999</v>
       </c>
       <c r="E7">
-        <v>8.7996599999999994</v>
+        <v>8.7817500000000006</v>
       </c>
       <c r="G7" s="1"/>
     </row>
@@ -554,16 +554,16 @@
         <v>1981</v>
       </c>
       <c r="B8">
-        <v>470.68099999999998</v>
+        <v>414.471</v>
       </c>
       <c r="C8">
-        <v>145.40199999999999</v>
+        <v>128.96299999999999</v>
       </c>
       <c r="D8">
-        <v>2079.5</v>
+        <v>1916.75</v>
       </c>
       <c r="E8">
-        <v>9.0241900000000008</v>
+        <v>9.0089100000000002</v>
       </c>
       <c r="H8" s="1"/>
     </row>
@@ -572,16 +572,16 @@
         <v>1982</v>
       </c>
       <c r="B9">
-        <v>494.00400000000002</v>
+        <v>442.64400000000001</v>
       </c>
       <c r="C9">
-        <v>140.05600000000001</v>
+        <v>124.673</v>
       </c>
       <c r="D9">
-        <v>2105.7399999999998</v>
+        <v>1947.66</v>
       </c>
       <c r="E9">
-        <v>11.830299999999999</v>
+        <v>11.7979</v>
       </c>
       <c r="H9" s="1"/>
     </row>
@@ -590,16 +590,16 @@
         <v>1983</v>
       </c>
       <c r="B10">
-        <v>575.19500000000005</v>
+        <v>525.47</v>
       </c>
       <c r="C10">
-        <v>143.18899999999999</v>
+        <v>128.62799999999999</v>
       </c>
       <c r="D10">
-        <v>1998.86</v>
+        <v>1837.78</v>
       </c>
       <c r="E10">
-        <v>13.5855</v>
+        <v>13.5395</v>
       </c>
       <c r="H10" s="1"/>
       <c r="L10" s="1"/>
@@ -650,16 +650,16 @@
         <v>1984</v>
       </c>
       <c r="B11">
-        <v>618.46299999999997</v>
+        <v>571.47500000000002</v>
       </c>
       <c r="C11">
-        <v>158.851</v>
+        <v>144.32900000000001</v>
       </c>
       <c r="D11">
-        <v>3985.1</v>
+        <v>3625.7</v>
       </c>
       <c r="E11">
-        <v>37.732100000000003</v>
+        <v>37.405700000000003</v>
       </c>
       <c r="H11" s="1"/>
     </row>
@@ -668,16 +668,16 @@
         <v>1985</v>
       </c>
       <c r="B12">
-        <v>803.61599999999999</v>
+        <v>748.97799999999995</v>
       </c>
       <c r="C12">
-        <v>156.559</v>
+        <v>142.416</v>
       </c>
       <c r="D12">
-        <v>3461.81</v>
+        <v>3124.67</v>
       </c>
       <c r="E12">
-        <v>18.752300000000002</v>
+        <v>18.732099999999999</v>
       </c>
       <c r="H12" s="1"/>
     </row>
@@ -686,16 +686,16 @@
         <v>1986</v>
       </c>
       <c r="B13">
-        <v>790.01800000000003</v>
+        <v>739.54300000000001</v>
       </c>
       <c r="C13">
-        <v>159.91800000000001</v>
+        <v>148.31899999999999</v>
       </c>
       <c r="D13">
-        <v>3228.16</v>
+        <v>2889.62</v>
       </c>
       <c r="E13">
-        <v>19.5991</v>
+        <v>19.578299999999999</v>
       </c>
       <c r="H13" s="1"/>
     </row>
@@ -704,16 +704,16 @@
         <v>1987</v>
       </c>
       <c r="B14">
-        <v>1038.33</v>
+        <v>979.56</v>
       </c>
       <c r="C14">
-        <v>183.79300000000001</v>
+        <v>173.923</v>
       </c>
       <c r="D14">
-        <v>5546.56</v>
+        <v>4915.76</v>
       </c>
       <c r="E14">
-        <v>40.880299999999998</v>
+        <v>40.8127</v>
       </c>
       <c r="H14" s="1"/>
     </row>
@@ -722,16 +722,16 @@
         <v>1988</v>
       </c>
       <c r="B15">
-        <v>1155.5899999999999</v>
+        <v>1089.56</v>
       </c>
       <c r="C15">
-        <v>185.55600000000001</v>
+        <v>178.01900000000001</v>
       </c>
       <c r="D15">
-        <v>9541.69</v>
+        <v>8408.61</v>
       </c>
       <c r="E15">
-        <v>86.692700000000002</v>
+        <v>86.476100000000002</v>
       </c>
       <c r="H15" s="1"/>
     </row>
@@ -740,16 +740,16 @@
         <v>1989</v>
       </c>
       <c r="B16">
-        <v>1207.74</v>
+        <v>1133.4100000000001</v>
       </c>
       <c r="C16">
-        <v>188.84399999999999</v>
+        <v>182.81299999999999</v>
       </c>
       <c r="D16">
-        <v>3630.4</v>
+        <v>3201.16</v>
       </c>
       <c r="E16">
-        <v>69.456999999999994</v>
+        <v>69.351399999999998</v>
       </c>
       <c r="H16" s="1"/>
     </row>
@@ -758,16 +758,16 @@
         <v>1990</v>
       </c>
       <c r="B17">
-        <v>1153.3800000000001</v>
+        <v>1084.7</v>
       </c>
       <c r="C17">
-        <v>200.15199999999999</v>
+        <v>195.036</v>
       </c>
       <c r="D17">
-        <v>2881.64</v>
+        <v>2539.85</v>
       </c>
       <c r="E17">
-        <v>35.343299999999999</v>
+        <v>35.321399999999997</v>
       </c>
       <c r="H17" s="1"/>
     </row>
@@ -776,16 +776,16 @@
         <v>1991</v>
       </c>
       <c r="B18">
-        <v>1250.74</v>
+        <v>1173.1300000000001</v>
       </c>
       <c r="C18">
-        <v>222.31800000000001</v>
+        <v>217.44900000000001</v>
       </c>
       <c r="D18">
-        <v>6781.89</v>
+        <v>5964.1</v>
       </c>
       <c r="E18">
-        <v>56.210599999999999</v>
+        <v>56.178100000000001</v>
       </c>
       <c r="H18" s="1"/>
     </row>
@@ -794,16 +794,16 @@
         <v>1992</v>
       </c>
       <c r="B19">
-        <v>1281.95</v>
+        <v>1201.06</v>
       </c>
       <c r="C19">
-        <v>243.13300000000001</v>
+        <v>237.911</v>
       </c>
       <c r="D19">
-        <v>3305.36</v>
+        <v>2911.76</v>
       </c>
       <c r="E19">
-        <v>52.856200000000001</v>
+        <v>52.854900000000001</v>
       </c>
       <c r="H19" s="1"/>
     </row>
@@ -812,16 +812,16 @@
         <v>1993</v>
       </c>
       <c r="B20">
-        <v>1562.74</v>
+        <v>1463.42</v>
       </c>
       <c r="C20">
-        <v>311.87900000000002</v>
+        <v>304.90199999999999</v>
       </c>
       <c r="D20">
-        <v>1888.6</v>
+        <v>1668.42</v>
       </c>
       <c r="E20">
-        <v>64.577600000000004</v>
+        <v>64.623199999999997</v>
       </c>
       <c r="H20" s="1"/>
     </row>
@@ -830,16 +830,16 @@
         <v>1994</v>
       </c>
       <c r="B21">
-        <v>1702.29</v>
+        <v>1593.47</v>
       </c>
       <c r="C21">
-        <v>369.35399999999998</v>
+        <v>359.827</v>
       </c>
       <c r="D21">
-        <v>2227.6</v>
+        <v>1971.62</v>
       </c>
       <c r="E21">
-        <v>59.918999999999997</v>
+        <v>60.021700000000003</v>
       </c>
       <c r="H21" s="1"/>
     </row>
@@ -848,16 +848,16 @@
         <v>1995</v>
       </c>
       <c r="B22">
-        <v>1711.42</v>
+        <v>1604.55</v>
       </c>
       <c r="C22">
-        <v>433.03800000000001</v>
+        <v>420.24700000000001</v>
       </c>
       <c r="D22">
-        <v>1409.2</v>
+        <v>1252.0899999999999</v>
       </c>
       <c r="E22">
-        <v>55.3429</v>
+        <v>55.437600000000003</v>
       </c>
       <c r="H22" s="1"/>
     </row>
@@ -866,16 +866,16 @@
         <v>1996</v>
       </c>
       <c r="B23">
-        <v>1820.56</v>
+        <v>1710.33</v>
       </c>
       <c r="C23">
-        <v>547.923</v>
+        <v>529.62199999999996</v>
       </c>
       <c r="D23">
-        <v>1503.41</v>
+        <v>1339.28</v>
       </c>
       <c r="E23">
-        <v>47.131999999999998</v>
+        <v>47.217199999999998</v>
       </c>
       <c r="H23" s="1"/>
     </row>
@@ -884,16 +884,16 @@
         <v>1997</v>
       </c>
       <c r="B24">
-        <v>1741.27</v>
+        <v>1641.42</v>
       </c>
       <c r="C24">
-        <v>601.32000000000005</v>
+        <v>581.64300000000003</v>
       </c>
       <c r="D24">
-        <v>1614.59</v>
+        <v>1442.2</v>
       </c>
       <c r="E24">
-        <v>68.327600000000004</v>
+        <v>68.536299999999997</v>
       </c>
       <c r="H24" s="1"/>
     </row>
@@ -902,16 +902,16 @@
         <v>1998</v>
       </c>
       <c r="B25">
-        <v>1585.61</v>
+        <v>1498.86</v>
       </c>
       <c r="C25">
-        <v>585.53700000000003</v>
+        <v>566.88300000000004</v>
       </c>
       <c r="D25">
-        <v>1022.66</v>
+        <v>917.23500000000001</v>
       </c>
       <c r="E25">
-        <v>33.607100000000003</v>
+        <v>33.683199999999999</v>
       </c>
       <c r="H25" s="1"/>
     </row>
@@ -920,16 +920,16 @@
         <v>1999</v>
       </c>
       <c r="B26">
-        <v>1400.1</v>
+        <v>1331.37</v>
       </c>
       <c r="C26">
-        <v>611.36</v>
+        <v>593.21699999999998</v>
       </c>
       <c r="D26">
-        <v>1710.82</v>
+        <v>1533.83</v>
       </c>
       <c r="E26">
-        <v>40.951500000000003</v>
+        <v>41.072899999999997</v>
       </c>
       <c r="H26" s="1"/>
     </row>
@@ -938,16 +938,16 @@
         <v>2000</v>
       </c>
       <c r="B27">
-        <v>1356.95</v>
+        <v>1294.8399999999999</v>
       </c>
       <c r="C27">
-        <v>642.36099999999999</v>
+        <v>624.13400000000001</v>
       </c>
       <c r="D27">
-        <v>1340.6</v>
+        <v>1201.4100000000001</v>
       </c>
       <c r="E27">
-        <v>49.353400000000001</v>
+        <v>49.537700000000001</v>
       </c>
       <c r="H27" s="1"/>
     </row>
@@ -956,16 +956,16 @@
         <v>2001</v>
       </c>
       <c r="B28">
-        <v>1431.4</v>
+        <v>1367.23</v>
       </c>
       <c r="C28">
-        <v>655.26300000000003</v>
+        <v>638.65200000000004</v>
       </c>
       <c r="D28">
-        <v>2769.65</v>
+        <v>2473.64</v>
       </c>
       <c r="E28">
-        <v>29.360700000000001</v>
+        <v>29.417999999999999</v>
       </c>
       <c r="H28" s="1"/>
     </row>
@@ -974,16 +974,16 @@
         <v>2002</v>
       </c>
       <c r="B29">
-        <v>1427.23</v>
+        <v>1365.73</v>
       </c>
       <c r="C29">
-        <v>658.74599999999998</v>
+        <v>644.01099999999997</v>
       </c>
       <c r="D29">
-        <v>4377.63</v>
+        <v>3902.44</v>
       </c>
       <c r="E29">
-        <v>41.624400000000001</v>
+        <v>41.754399999999997</v>
       </c>
       <c r="H29" s="1"/>
     </row>
@@ -992,16 +992,16 @@
         <v>2003</v>
       </c>
       <c r="B30">
-        <v>1481.92</v>
+        <v>1418.69</v>
       </c>
       <c r="C30">
-        <v>663.41399999999999</v>
+        <v>650.9</v>
       </c>
       <c r="D30">
-        <v>5070.54</v>
+        <v>4513.92</v>
       </c>
       <c r="E30">
-        <v>35.922800000000002</v>
+        <v>36.021599999999999</v>
       </c>
       <c r="H30" s="1"/>
     </row>
@@ -1010,16 +1010,16 @@
         <v>2004</v>
       </c>
       <c r="B31">
-        <v>1761.77</v>
+        <v>1675.15</v>
       </c>
       <c r="C31">
-        <v>645.76499999999999</v>
+        <v>634.87800000000004</v>
       </c>
       <c r="D31">
-        <v>4181.18</v>
+        <v>3721.76</v>
       </c>
       <c r="E31">
-        <v>48.405500000000004</v>
+        <v>48.593499999999999</v>
       </c>
       <c r="H31" s="1"/>
     </row>
@@ -1028,16 +1028,16 @@
         <v>2005</v>
       </c>
       <c r="B32">
-        <v>1576.9</v>
+        <v>1500.9</v>
       </c>
       <c r="C32">
-        <v>538.55399999999997</v>
+        <v>531.99099999999999</v>
       </c>
       <c r="D32">
-        <v>3756.2</v>
+        <v>3348.82</v>
       </c>
       <c r="E32">
-        <v>37.234400000000001</v>
+        <v>37.349499999999999</v>
       </c>
       <c r="H32" s="1"/>
     </row>
@@ -1046,16 +1046,16 @@
         <v>2006</v>
       </c>
       <c r="B33">
-        <v>1433.05</v>
+        <v>1366.94</v>
       </c>
       <c r="C33">
-        <v>483.59500000000003</v>
+        <v>480.23200000000003</v>
       </c>
       <c r="D33">
-        <v>4627.0200000000004</v>
+        <v>4135.78</v>
       </c>
       <c r="E33">
-        <v>36.370199999999997</v>
+        <v>36.4895</v>
       </c>
       <c r="H33" s="1"/>
     </row>
@@ -1064,16 +1064,16 @@
         <v>2007</v>
       </c>
       <c r="B34">
-        <v>1418.96</v>
+        <v>1354.31</v>
       </c>
       <c r="C34">
-        <v>455.548</v>
+        <v>453.416</v>
       </c>
       <c r="D34">
-        <v>1360.58</v>
+        <v>1224.24</v>
       </c>
       <c r="E34">
-        <v>37.0961</v>
+        <v>37.217300000000002</v>
       </c>
       <c r="H34" s="1"/>
     </row>
@@ -1082,16 +1082,16 @@
         <v>2008</v>
       </c>
       <c r="B35">
-        <v>1468</v>
+        <v>1400.55</v>
       </c>
       <c r="C35">
-        <v>443.50599999999997</v>
+        <v>440.98700000000002</v>
       </c>
       <c r="D35">
-        <v>403.38600000000002</v>
+        <v>367.46</v>
       </c>
       <c r="E35">
-        <v>51.306800000000003</v>
+        <v>51.555500000000002</v>
       </c>
       <c r="H35" s="1"/>
     </row>
@@ -1100,16 +1100,16 @@
         <v>2009</v>
       </c>
       <c r="B36">
-        <v>1393.44</v>
+        <v>1330.13</v>
       </c>
       <c r="C36">
-        <v>402.286</v>
+        <v>399.97699999999998</v>
       </c>
       <c r="D36">
-        <v>344.85500000000002</v>
+        <v>316.55</v>
       </c>
       <c r="E36">
-        <v>48.773200000000003</v>
+        <v>48.994599999999998</v>
       </c>
       <c r="H36" s="1"/>
     </row>
@@ -1118,16 +1118,16 @@
         <v>2010</v>
       </c>
       <c r="B37">
-        <v>1468.27</v>
+        <v>1401.7</v>
       </c>
       <c r="C37">
-        <v>439.35899999999998</v>
+        <v>434.41300000000001</v>
       </c>
       <c r="D37">
-        <v>254.75299999999999</v>
+        <v>235.50800000000001</v>
       </c>
       <c r="E37">
-        <v>53.298299999999998</v>
+        <v>53.554299999999998</v>
       </c>
       <c r="H37" s="1"/>
     </row>
@@ -1136,16 +1136,16 @@
         <v>2011</v>
       </c>
       <c r="B38">
-        <v>1661.8</v>
+        <v>1586.57</v>
       </c>
       <c r="C38">
-        <v>516.38499999999999</v>
+        <v>507.52499999999998</v>
       </c>
       <c r="D38">
-        <v>334.02800000000002</v>
+        <v>308.30799999999999</v>
       </c>
       <c r="E38">
-        <v>60.702100000000002</v>
+        <v>60.984999999999999</v>
       </c>
       <c r="H38" s="1"/>
     </row>
@@ -1154,16 +1154,16 @@
         <v>2012</v>
       </c>
       <c r="B39">
-        <v>1504.86</v>
+        <v>1443.27</v>
       </c>
       <c r="C39">
-        <v>568.06100000000004</v>
+        <v>556.77499999999998</v>
       </c>
       <c r="D39">
-        <v>412.79</v>
+        <v>382.04500000000002</v>
       </c>
       <c r="E39">
-        <v>76.154399999999995</v>
+        <v>76.559700000000007</v>
       </c>
       <c r="H39" s="1"/>
     </row>
@@ -1172,16 +1172,16 @@
         <v>2013</v>
       </c>
       <c r="B40">
-        <v>1363.23</v>
+        <v>1311.75</v>
       </c>
       <c r="C40">
-        <v>593.66</v>
+        <v>580.71799999999996</v>
       </c>
       <c r="D40">
-        <v>402.23500000000001</v>
+        <v>374.553</v>
       </c>
       <c r="E40">
-        <v>59.792400000000001</v>
+        <v>60.018099999999997</v>
       </c>
       <c r="H40" s="1"/>
     </row>
@@ -1190,16 +1190,16 @@
         <v>2014</v>
       </c>
       <c r="B41">
-        <v>1191.54</v>
+        <v>1152.21</v>
       </c>
       <c r="C41">
-        <v>608.99599999999998</v>
+        <v>596.29999999999995</v>
       </c>
       <c r="D41">
-        <v>289.714</v>
+        <v>271.37799999999999</v>
       </c>
       <c r="E41">
-        <v>51.740600000000001</v>
+        <v>51.915700000000001</v>
       </c>
       <c r="H41" s="1"/>
     </row>
@@ -1208,16 +1208,16 @@
         <v>2015</v>
       </c>
       <c r="B42">
-        <v>1176.08</v>
+        <v>1141.51</v>
       </c>
       <c r="C42">
-        <v>631.53300000000002</v>
+        <v>619.71500000000003</v>
       </c>
       <c r="D42">
-        <v>1137.6199999999999</v>
+        <v>1056.8</v>
       </c>
       <c r="E42">
-        <v>45.512799999999999</v>
+        <v>45.662999999999997</v>
       </c>
       <c r="H42" s="1"/>
     </row>
@@ -1226,16 +1226,16 @@
         <v>2016</v>
       </c>
       <c r="B43">
-        <v>1009.33</v>
+        <v>984.37599999999998</v>
       </c>
       <c r="C43">
-        <v>556.82899999999995</v>
+        <v>549.38599999999997</v>
       </c>
       <c r="D43">
-        <v>1912.84</v>
+        <v>1764.33</v>
       </c>
       <c r="E43">
-        <v>45.058</v>
+        <v>45.186599999999999</v>
       </c>
       <c r="H43" s="1"/>
     </row>
@@ -1244,16 +1244,16 @@
         <v>2017</v>
       </c>
       <c r="B44">
-        <v>896.64300000000003</v>
+        <v>878.125</v>
       </c>
       <c r="C44">
-        <v>491.26499999999999</v>
+        <v>487.75799999999998</v>
       </c>
       <c r="D44">
-        <v>2146.81</v>
+        <v>1965.68</v>
       </c>
       <c r="E44">
-        <v>35.115400000000001</v>
+        <v>35.189300000000003</v>
       </c>
       <c r="H44" s="1"/>
     </row>
@@ -1262,16 +1262,16 @@
         <v>2018</v>
       </c>
       <c r="B45">
-        <v>843.89099999999996</v>
+        <v>827.529</v>
       </c>
       <c r="C45">
-        <v>415.68200000000002</v>
+        <v>415.495</v>
       </c>
       <c r="D45">
-        <v>1781.76</v>
+        <v>1628.32</v>
       </c>
       <c r="E45">
-        <v>28.218599999999999</v>
+        <v>28.260999999999999</v>
       </c>
       <c r="H45" s="1"/>
     </row>
@@ -1280,16 +1280,16 @@
         <v>2019</v>
       </c>
       <c r="B46">
-        <v>879.02800000000002</v>
+        <v>860.53300000000002</v>
       </c>
       <c r="C46">
-        <v>363.65100000000001</v>
+        <v>365.93900000000002</v>
       </c>
       <c r="D46">
-        <v>1698.71</v>
+        <v>1571.09</v>
       </c>
       <c r="E46">
-        <v>25.854900000000001</v>
+        <v>25.892800000000001</v>
       </c>
       <c r="H46" s="1"/>
     </row>
@@ -1298,16 +1298,16 @@
         <v>2020</v>
       </c>
       <c r="B47">
-        <v>908.42399999999998</v>
+        <v>888.68600000000004</v>
       </c>
       <c r="C47">
-        <v>313.97699999999998</v>
+        <v>318.46199999999999</v>
       </c>
       <c r="D47">
-        <v>1609.75</v>
+        <v>1523.98</v>
       </c>
       <c r="E47">
-        <v>25.988399999999999</v>
+        <v>26.0152</v>
       </c>
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
@@ -1315,16 +1315,16 @@
         <v>2021</v>
       </c>
       <c r="B48">
-        <v>940.83799999999997</v>
+        <v>920.86500000000001</v>
       </c>
       <c r="C48">
-        <v>271.46899999999999</v>
+        <v>277.30399999999997</v>
       </c>
       <c r="D48">
-        <v>1062.53</v>
+        <v>1102.73</v>
       </c>
       <c r="E48">
-        <v>14.404299999999999</v>
+        <v>14.410500000000001</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -1332,16 +1332,16 @@
         <v>2022</v>
       </c>
       <c r="B49">
-        <v>1018.1</v>
+        <v>998.39</v>
       </c>
       <c r="C49">
-        <v>254.077</v>
+        <v>260.44099999999997</v>
       </c>
       <c r="D49">
-        <v>758.625</v>
+        <v>989.01400000000001</v>
       </c>
       <c r="E49">
-        <v>18.401499999999999</v>
+        <v>18.407499999999999</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -1349,16 +1349,16 @@
         <v>2023</v>
       </c>
       <c r="B50">
-        <v>1033.19</v>
+        <v>1020.84</v>
       </c>
       <c r="C50">
-        <v>247.87299999999999</v>
+        <v>254.16</v>
       </c>
       <c r="D50">
-        <v>948.88800000000003</v>
+        <v>1384.13</v>
       </c>
       <c r="E50">
-        <v>27.203199999999999</v>
+        <v>27.2119</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -1366,16 +1366,16 @@
         <v>2024</v>
       </c>
       <c r="B51">
-        <v>1048.79</v>
+        <v>1051.04</v>
       </c>
       <c r="C51">
-        <v>266.26400000000001</v>
+        <v>271.988</v>
       </c>
       <c r="D51">
-        <v>981.02499999999998</v>
+        <v>1462.25</v>
       </c>
       <c r="E51">
-        <v>27.336400000000001</v>
+        <v>27.3398</v>
       </c>
     </row>
   </sheetData>
@@ -1387,8 +1387,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6C3CC098-F8E2-4D37-ABCD-D1C33B6F7A68}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B51"/>
+    <sheetView topLeftCell="A29" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1415,16 +1415,16 @@
         <v>1975</v>
       </c>
       <c r="B2">
-        <v>582.07299999999998</v>
+        <v>485.87299999999999</v>
       </c>
       <c r="C2">
-        <v>48.333300000000001</v>
+        <v>39.598399999999998</v>
       </c>
       <c r="D2">
-        <v>493.14699999999999</v>
+        <v>412.90499999999997</v>
       </c>
       <c r="E2">
-        <v>687.03399999999999</v>
+        <v>571.73500000000001</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -1432,16 +1432,16 @@
         <v>1976</v>
       </c>
       <c r="B3">
-        <v>1364.42</v>
+        <v>1189.76</v>
       </c>
       <c r="C3">
-        <v>94.441599999999994</v>
+        <v>80.567499999999995</v>
       </c>
       <c r="D3">
-        <v>1188.23</v>
+        <v>1039.22</v>
       </c>
       <c r="E3">
-        <v>1566.74</v>
+        <v>1362.1</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -1449,16 +1449,16 @@
         <v>1977</v>
       </c>
       <c r="B4">
-        <v>724.01300000000003</v>
+        <v>658.94100000000003</v>
       </c>
       <c r="C4">
-        <v>57.231499999999997</v>
+        <v>51.743200000000002</v>
       </c>
       <c r="D4">
-        <v>618.29200000000003</v>
+        <v>563.30700000000002</v>
       </c>
       <c r="E4">
-        <v>847.81200000000001</v>
+        <v>770.81</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -1466,16 +1466,16 @@
         <v>1978</v>
       </c>
       <c r="B5">
-        <v>1033.6600000000001</v>
+        <v>959.24</v>
       </c>
       <c r="C5">
-        <v>77.278700000000001</v>
+        <v>70.550200000000004</v>
       </c>
       <c r="D5">
-        <v>890.29100000000005</v>
+        <v>828.19</v>
       </c>
       <c r="E5">
-        <v>1200.1199999999999</v>
+        <v>1111.03</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -1483,16 +1483,16 @@
         <v>1979</v>
       </c>
       <c r="B6">
-        <v>947.46100000000001</v>
+        <v>876.851</v>
       </c>
       <c r="C6">
-        <v>70.550299999999993</v>
+        <v>64.132900000000006</v>
       </c>
       <c r="D6">
-        <v>816.53200000000004</v>
+        <v>757.673</v>
       </c>
       <c r="E6">
-        <v>1099.3800000000001</v>
+        <v>1014.77</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -1500,16 +1500,16 @@
         <v>1980</v>
       </c>
       <c r="B7">
-        <v>1206.3399999999999</v>
+        <v>1111.1099999999999</v>
       </c>
       <c r="C7">
-        <v>82.4101</v>
+        <v>74.407799999999995</v>
       </c>
       <c r="D7">
-        <v>1052.45</v>
+        <v>971.97500000000002</v>
       </c>
       <c r="E7">
-        <v>1382.73</v>
+        <v>1270.1600000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -1517,16 +1517,16 @@
         <v>1981</v>
       </c>
       <c r="B8">
-        <v>2079.5</v>
+        <v>1916.75</v>
       </c>
       <c r="C8">
-        <v>126.167</v>
+        <v>113.605</v>
       </c>
       <c r="D8">
-        <v>1842.08</v>
+        <v>1702.67</v>
       </c>
       <c r="E8">
-        <v>2347.52</v>
+        <v>2157.75</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -1534,16 +1534,16 @@
         <v>1982</v>
       </c>
       <c r="B9">
-        <v>2105.7399999999998</v>
+        <v>1947.66</v>
       </c>
       <c r="C9">
-        <v>130.69399999999999</v>
+        <v>118.146</v>
       </c>
       <c r="D9">
-        <v>1860.15</v>
+        <v>1725.33</v>
       </c>
       <c r="E9">
-        <v>2383.7600000000002</v>
+        <v>2198.64</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -1551,16 +1551,16 @@
         <v>1983</v>
       </c>
       <c r="B10">
-        <v>1998.86</v>
+        <v>1837.78</v>
       </c>
       <c r="C10">
-        <v>129.22300000000001</v>
+        <v>116.11799999999999</v>
       </c>
       <c r="D10">
-        <v>1756.66</v>
+        <v>1619.83</v>
       </c>
       <c r="E10">
-        <v>2274.4499999999998</v>
+        <v>2085.0700000000002</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -1568,16 +1568,16 @@
         <v>1984</v>
       </c>
       <c r="B11">
-        <v>3985.1</v>
+        <v>3625.7</v>
       </c>
       <c r="C11">
-        <v>240.31399999999999</v>
+        <v>213.26</v>
       </c>
       <c r="D11">
-        <v>3532.71</v>
+        <v>3223.64</v>
       </c>
       <c r="E11">
-        <v>4495.42</v>
+        <v>4077.91</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -1585,16 +1585,16 @@
         <v>1985</v>
       </c>
       <c r="B12">
-        <v>3461.81</v>
+        <v>3124.67</v>
       </c>
       <c r="C12">
-        <v>230.29599999999999</v>
+        <v>204.7</v>
       </c>
       <c r="D12">
-        <v>3030.99</v>
+        <v>2741.34</v>
       </c>
       <c r="E12">
-        <v>3953.87</v>
+        <v>3561.6</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -1602,16 +1602,16 @@
         <v>1986</v>
       </c>
       <c r="B13">
-        <v>3228.16</v>
+        <v>2889.62</v>
       </c>
       <c r="C13">
-        <v>241.422</v>
+        <v>213.76400000000001</v>
       </c>
       <c r="D13">
-        <v>2780.27</v>
+        <v>2492.7199999999998</v>
       </c>
       <c r="E13">
-        <v>3748.21</v>
+        <v>3349.72</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -1619,16 +1619,16 @@
         <v>1987</v>
       </c>
       <c r="B14">
-        <v>5546.56</v>
+        <v>4915.76</v>
       </c>
       <c r="C14">
-        <v>405.84199999999998</v>
+        <v>355.85599999999999</v>
       </c>
       <c r="D14">
-        <v>4792.41</v>
+        <v>4253.9799999999996</v>
       </c>
       <c r="E14">
-        <v>6419.39</v>
+        <v>5680.5</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -1636,16 +1636,16 @@
         <v>1988</v>
       </c>
       <c r="B15">
-        <v>9541.69</v>
+        <v>8408.61</v>
       </c>
       <c r="C15">
-        <v>657.40800000000002</v>
+        <v>572.43200000000002</v>
       </c>
       <c r="D15">
-        <v>8314.7999999999993</v>
+        <v>7339.42</v>
       </c>
       <c r="E15">
-        <v>10949.6</v>
+        <v>9633.5499999999993</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -1653,16 +1653,16 @@
         <v>1989</v>
       </c>
       <c r="B16">
-        <v>3630.4</v>
+        <v>3201.16</v>
       </c>
       <c r="C16">
-        <v>283.75099999999998</v>
+        <v>247.67699999999999</v>
       </c>
       <c r="D16">
-        <v>3105.77</v>
+        <v>2742.87</v>
       </c>
       <c r="E16">
-        <v>4243.66</v>
+        <v>3736.04</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1670,16 +1670,16 @@
         <v>1990</v>
       </c>
       <c r="B17">
-        <v>2881.64</v>
+        <v>2539.85</v>
       </c>
       <c r="C17">
-        <v>233.893</v>
+        <v>204.11</v>
       </c>
       <c r="D17">
-        <v>2450.5</v>
+        <v>2163.31</v>
       </c>
       <c r="E17">
-        <v>3388.64</v>
+        <v>2981.94</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -1687,16 +1687,16 @@
         <v>1991</v>
       </c>
       <c r="B18">
-        <v>6781.89</v>
+        <v>5964.1</v>
       </c>
       <c r="C18">
-        <v>474.976</v>
+        <v>412.49400000000003</v>
       </c>
       <c r="D18">
-        <v>5896.48</v>
+        <v>5194.4799999999996</v>
       </c>
       <c r="E18">
-        <v>7800.25</v>
+        <v>6847.74</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -1704,16 +1704,16 @@
         <v>1992</v>
       </c>
       <c r="B19">
-        <v>3305.36</v>
+        <v>2911.76</v>
       </c>
       <c r="C19">
-        <v>252.30799999999999</v>
+        <v>219.82300000000001</v>
       </c>
       <c r="D19">
-        <v>2838</v>
+        <v>2504.23</v>
       </c>
       <c r="E19">
-        <v>3849.67</v>
+        <v>3385.61</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -1721,16 +1721,16 @@
         <v>1993</v>
       </c>
       <c r="B20">
-        <v>1888.6</v>
+        <v>1668.42</v>
       </c>
       <c r="C20">
-        <v>157.66499999999999</v>
+        <v>137.93299999999999</v>
       </c>
       <c r="D20">
-        <v>1598.65</v>
+        <v>1414.55</v>
       </c>
       <c r="E20">
-        <v>2231.13</v>
+        <v>1967.85</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -1738,16 +1738,16 @@
         <v>1994</v>
       </c>
       <c r="B21">
-        <v>2227.6</v>
+        <v>1971.62</v>
       </c>
       <c r="C21">
-        <v>174.03100000000001</v>
+        <v>152.392</v>
       </c>
       <c r="D21">
-        <v>1905.82</v>
+        <v>1689.62</v>
       </c>
       <c r="E21">
-        <v>2603.71</v>
+        <v>2300.69</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1755,16 +1755,16 @@
         <v>1995</v>
       </c>
       <c r="B22">
-        <v>1409.2</v>
+        <v>1252.0899999999999</v>
       </c>
       <c r="C22">
-        <v>119.152</v>
+        <v>104.815</v>
       </c>
       <c r="D22">
-        <v>1190.32</v>
+        <v>1059.3800000000001</v>
       </c>
       <c r="E22">
-        <v>1668.34</v>
+        <v>1479.86</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1772,16 +1772,16 @@
         <v>1996</v>
       </c>
       <c r="B23">
-        <v>1503.41</v>
+        <v>1339.28</v>
       </c>
       <c r="C23">
-        <v>121.979</v>
+        <v>107.536</v>
       </c>
       <c r="D23">
-        <v>1278.56</v>
+        <v>1140.8800000000001</v>
       </c>
       <c r="E23">
-        <v>1767.81</v>
+        <v>1572.18</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1789,16 +1789,16 @@
         <v>1997</v>
       </c>
       <c r="B24">
-        <v>1614.59</v>
+        <v>1442.2</v>
       </c>
       <c r="C24">
-        <v>126.377</v>
+        <v>111.631</v>
       </c>
       <c r="D24">
-        <v>1380.96</v>
+        <v>1235.6400000000001</v>
       </c>
       <c r="E24">
-        <v>1887.75</v>
+        <v>1683.28</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1806,16 +1806,16 @@
         <v>1998</v>
       </c>
       <c r="B25">
-        <v>1022.66</v>
+        <v>917.23500000000001</v>
       </c>
       <c r="C25">
-        <v>88.237399999999994</v>
+        <v>78.366299999999995</v>
       </c>
       <c r="D25">
-        <v>860.84500000000003</v>
+        <v>773.40300000000002</v>
       </c>
       <c r="E25">
-        <v>1214.8800000000001</v>
+        <v>1087.82</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1823,16 +1823,16 @@
         <v>1999</v>
       </c>
       <c r="B26">
-        <v>1710.82</v>
+        <v>1533.83</v>
       </c>
       <c r="C26">
-        <v>129.251</v>
+        <v>114.422</v>
       </c>
       <c r="D26">
-        <v>1471.21</v>
+        <v>1321.51</v>
       </c>
       <c r="E26">
-        <v>1989.44</v>
+        <v>1780.26</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -1840,16 +1840,16 @@
         <v>2000</v>
       </c>
       <c r="B27">
-        <v>1340.6</v>
+        <v>1201.4100000000001</v>
       </c>
       <c r="C27">
-        <v>108.121</v>
+        <v>95.674700000000001</v>
       </c>
       <c r="D27">
-        <v>1141.2</v>
+        <v>1024.78</v>
       </c>
       <c r="E27">
-        <v>1574.85</v>
+        <v>1408.48</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -1857,16 +1857,16 @@
         <v>2001</v>
       </c>
       <c r="B28">
-        <v>2769.65</v>
+        <v>2473.64</v>
       </c>
       <c r="C28">
-        <v>195.12700000000001</v>
+        <v>171.535</v>
       </c>
       <c r="D28">
-        <v>2406.06</v>
+        <v>2153.66</v>
       </c>
       <c r="E28">
-        <v>3188.18</v>
+        <v>2841.17</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1874,16 +1874,16 @@
         <v>2002</v>
       </c>
       <c r="B29">
-        <v>4377.63</v>
+        <v>3902.44</v>
       </c>
       <c r="C29">
-        <v>293.52300000000002</v>
+        <v>257.06599999999997</v>
       </c>
       <c r="D29">
-        <v>3828.82</v>
+        <v>3421.22</v>
       </c>
       <c r="E29">
-        <v>5005.1000000000004</v>
+        <v>4451.34</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1891,16 +1891,16 @@
         <v>2003</v>
       </c>
       <c r="B30">
-        <v>5070.54</v>
+        <v>4513.92</v>
       </c>
       <c r="C30">
-        <v>339.62099999999998</v>
+        <v>296.85399999999998</v>
       </c>
       <c r="D30">
-        <v>4435.49</v>
+        <v>3958.16</v>
       </c>
       <c r="E30">
-        <v>5796.51</v>
+        <v>5147.71</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -1908,16 +1908,16 @@
         <v>2004</v>
       </c>
       <c r="B31">
-        <v>4181.18</v>
+        <v>3721.76</v>
       </c>
       <c r="C31">
-        <v>289.17399999999998</v>
+        <v>253.03399999999999</v>
       </c>
       <c r="D31">
-        <v>3641.65</v>
+        <v>3249.1</v>
       </c>
       <c r="E31">
-        <v>4800.6499999999996</v>
+        <v>4263.18</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -1925,16 +1925,16 @@
         <v>2005</v>
       </c>
       <c r="B32">
-        <v>3756.2</v>
+        <v>3348.82</v>
       </c>
       <c r="C32">
-        <v>264.363</v>
+        <v>232.005</v>
       </c>
       <c r="D32">
-        <v>3263.57</v>
+        <v>2916</v>
       </c>
       <c r="E32">
-        <v>4323.2</v>
+        <v>3845.88</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -1942,16 +1942,16 @@
         <v>2006</v>
       </c>
       <c r="B33">
-        <v>4627.0200000000004</v>
+        <v>4135.78</v>
       </c>
       <c r="C33">
-        <v>317.72800000000001</v>
+        <v>279.858</v>
       </c>
       <c r="D33">
-        <v>4033.92</v>
+        <v>3612.85</v>
       </c>
       <c r="E33">
-        <v>5307.32</v>
+        <v>4734.41</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -1959,16 +1959,16 @@
         <v>2007</v>
       </c>
       <c r="B34">
-        <v>1360.58</v>
+        <v>1224.24</v>
       </c>
       <c r="C34">
-        <v>114.437</v>
+        <v>102.10899999999999</v>
       </c>
       <c r="D34">
-        <v>1150.26</v>
+        <v>1036.44</v>
       </c>
       <c r="E34">
-        <v>1609.35</v>
+        <v>1446.06</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1976,16 +1976,16 @@
         <v>2008</v>
       </c>
       <c r="B35">
-        <v>403.38600000000002</v>
+        <v>367.46</v>
       </c>
       <c r="C35">
-        <v>48.761099999999999</v>
+        <v>44.103499999999997</v>
       </c>
       <c r="D35">
-        <v>317.03500000000003</v>
+        <v>289.28899999999999</v>
       </c>
       <c r="E35">
-        <v>513.25699999999995</v>
+        <v>466.75400000000002</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -1993,16 +1993,16 @@
         <v>2009</v>
       </c>
       <c r="B36">
-        <v>344.85500000000002</v>
+        <v>316.55</v>
       </c>
       <c r="C36">
-        <v>42.574599999999997</v>
+        <v>38.748699999999999</v>
       </c>
       <c r="D36">
-        <v>269.65499999999997</v>
+        <v>248.036</v>
       </c>
       <c r="E36">
-        <v>441.02600000000001</v>
+        <v>403.99099999999999</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2010,16 +2010,16 @@
         <v>2010</v>
       </c>
       <c r="B37">
-        <v>254.75299999999999</v>
+        <v>235.50800000000001</v>
       </c>
       <c r="C37">
-        <v>34.067</v>
+        <v>31.138300000000001</v>
       </c>
       <c r="D37">
-        <v>195.20099999999999</v>
+        <v>180.99199999999999</v>
       </c>
       <c r="E37">
-        <v>332.47399999999999</v>
+        <v>306.44400000000002</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2027,16 +2027,16 @@
         <v>2011</v>
       </c>
       <c r="B38">
-        <v>334.02800000000002</v>
+        <v>308.30799999999999</v>
       </c>
       <c r="C38">
-        <v>39.515300000000003</v>
+        <v>36.107100000000003</v>
       </c>
       <c r="D38">
-        <v>263.86799999999999</v>
+        <v>244.12200000000001</v>
       </c>
       <c r="E38">
-        <v>422.84399999999999</v>
+        <v>389.36900000000003</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2044,16 +2044,16 @@
         <v>2012</v>
       </c>
       <c r="B39">
-        <v>412.79</v>
+        <v>382.04500000000002</v>
       </c>
       <c r="C39">
-        <v>44.2774</v>
+        <v>40.703699999999998</v>
       </c>
       <c r="D39">
-        <v>333.29399999999998</v>
+        <v>308.91199999999998</v>
       </c>
       <c r="E39">
-        <v>511.24700000000001</v>
+        <v>472.49200000000002</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2061,16 +2061,16 @@
         <v>2013</v>
       </c>
       <c r="B40">
-        <v>402.23500000000001</v>
+        <v>374.553</v>
       </c>
       <c r="C40">
-        <v>42.738799999999998</v>
+        <v>39.5503</v>
       </c>
       <c r="D40">
-        <v>325.423</v>
+        <v>303.42500000000001</v>
       </c>
       <c r="E40">
-        <v>497.17700000000002</v>
+        <v>462.35599999999999</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2078,16 +2078,16 @@
         <v>2014</v>
       </c>
       <c r="B41">
-        <v>289.714</v>
+        <v>271.37799999999999</v>
       </c>
       <c r="C41">
-        <v>34.908299999999997</v>
+        <v>32.4437</v>
       </c>
       <c r="D41">
-        <v>227.87100000000001</v>
+        <v>213.84700000000001</v>
       </c>
       <c r="E41">
-        <v>368.34199999999998</v>
+        <v>344.38799999999998</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2095,16 +2095,16 @@
         <v>2015</v>
       </c>
       <c r="B42">
-        <v>1137.6199999999999</v>
+        <v>1056.8</v>
       </c>
       <c r="C42">
-        <v>95.679500000000004</v>
+        <v>87.802899999999994</v>
       </c>
       <c r="D42">
-        <v>961.77099999999996</v>
+        <v>895.26</v>
       </c>
       <c r="E42">
-        <v>1345.61</v>
+        <v>1247.48</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2112,16 +2112,16 @@
         <v>2016</v>
       </c>
       <c r="B43">
-        <v>1912.84</v>
+        <v>1764.33</v>
       </c>
       <c r="C43">
-        <v>154.142</v>
+        <v>140.10400000000001</v>
       </c>
       <c r="D43">
-        <v>1628.54</v>
+        <v>1505.62</v>
       </c>
       <c r="E43">
-        <v>2246.77</v>
+        <v>2067.5100000000002</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -2129,16 +2129,16 @@
         <v>2017</v>
       </c>
       <c r="B44">
-        <v>2146.81</v>
+        <v>1965.68</v>
       </c>
       <c r="C44">
-        <v>194.60300000000001</v>
+        <v>175.53299999999999</v>
       </c>
       <c r="D44">
-        <v>1791.51</v>
+        <v>1644.76</v>
       </c>
       <c r="E44">
-        <v>2572.58</v>
+        <v>2349.2199999999998</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -2146,16 +2146,16 @@
         <v>2018</v>
       </c>
       <c r="B45">
-        <v>1781.76</v>
+        <v>1628.32</v>
       </c>
       <c r="C45">
-        <v>217.495</v>
+        <v>196.96899999999999</v>
       </c>
       <c r="D45">
-        <v>1397.06</v>
+        <v>1279.53</v>
       </c>
       <c r="E45">
-        <v>2272.4</v>
+        <v>2072.17</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -2163,16 +2163,16 @@
         <v>2019</v>
       </c>
       <c r="B46">
-        <v>1698.71</v>
+        <v>1571.09</v>
       </c>
       <c r="C46">
-        <v>269.93299999999999</v>
+        <v>246.44499999999999</v>
       </c>
       <c r="D46">
-        <v>1238.67</v>
+        <v>1150.21</v>
       </c>
       <c r="E46">
-        <v>2329.61</v>
+        <v>2145.96</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -2180,16 +2180,16 @@
         <v>2020</v>
       </c>
       <c r="B47">
-        <v>1609.75</v>
+        <v>1523.98</v>
       </c>
       <c r="C47">
-        <v>353.267</v>
+        <v>327.51299999999998</v>
       </c>
       <c r="D47">
-        <v>1043.23</v>
+        <v>996.35799999999995</v>
       </c>
       <c r="E47">
-        <v>2483.92</v>
+        <v>2330.9899999999998</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -2197,16 +2197,16 @@
         <v>2021</v>
       </c>
       <c r="B48">
-        <v>1062.53</v>
+        <v>1102.73</v>
       </c>
       <c r="C48">
-        <v>404.31599999999997</v>
+        <v>401.166</v>
       </c>
       <c r="D48">
-        <v>509.255</v>
+        <v>544.81200000000001</v>
       </c>
       <c r="E48">
-        <v>2216.92</v>
+        <v>2231.9699999999998</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -2214,16 +2214,16 @@
         <v>2022</v>
       </c>
       <c r="B49">
-        <v>758.625</v>
+        <v>989.01400000000001</v>
       </c>
       <c r="C49">
-        <v>465.53199999999998</v>
+        <v>576.02599999999995</v>
       </c>
       <c r="D49">
-        <v>244.90100000000001</v>
+        <v>335.56299999999999</v>
       </c>
       <c r="E49">
-        <v>2349.98</v>
+        <v>2914.95</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -2231,16 +2231,16 @@
         <v>2023</v>
       </c>
       <c r="B50">
-        <v>948.88800000000003</v>
+        <v>1384.13</v>
       </c>
       <c r="C50">
-        <v>660.77200000000005</v>
+        <v>952.01099999999997</v>
       </c>
       <c r="D50">
-        <v>269.81400000000002</v>
+        <v>398.64299999999997</v>
       </c>
       <c r="E50">
-        <v>3337.07</v>
+        <v>4805.8100000000004</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -2248,16 +2248,16 @@
         <v>2024</v>
       </c>
       <c r="B51">
-        <v>981.02499999999998</v>
+        <v>1462.25</v>
       </c>
       <c r="C51">
-        <v>701.505</v>
+        <v>1047.72</v>
       </c>
       <c r="D51">
-        <v>271.32400000000001</v>
+        <v>403.56099999999998</v>
       </c>
       <c r="E51">
-        <v>3547.09</v>
+        <v>5298.29</v>
       </c>
     </row>
   </sheetData>
@@ -2270,7 +2270,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B51"/>
+      <selection activeCell="B2" sqref="B2:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2297,16 +2297,16 @@
         <v>1975</v>
       </c>
       <c r="B2">
-        <v>63.967199999999998</v>
+        <v>60.297600000000003</v>
       </c>
       <c r="C2">
-        <v>5.1294899999999997</v>
+        <v>4.4264799999999997</v>
       </c>
       <c r="D2">
-        <v>54.502600000000001</v>
+        <v>52.074100000000001</v>
       </c>
       <c r="E2">
-        <v>75.075400000000002</v>
+        <v>69.819699999999997</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -2314,16 +2314,16 @@
         <v>1976</v>
       </c>
       <c r="B3">
-        <v>69.837000000000003</v>
+        <v>63.517699999999998</v>
       </c>
       <c r="C3">
-        <v>6.04453</v>
+        <v>4.8530199999999999</v>
       </c>
       <c r="D3">
-        <v>58.755400000000002</v>
+        <v>54.5289</v>
       </c>
       <c r="E3">
-        <v>83.008700000000005</v>
+        <v>73.988100000000003</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -2331,16 +2331,16 @@
         <v>1977</v>
       </c>
       <c r="B4">
-        <v>81.614599999999996</v>
+        <v>72.361999999999995</v>
       </c>
       <c r="C4">
-        <v>6.9864800000000002</v>
+        <v>5.4570400000000001</v>
       </c>
       <c r="D4">
-        <v>68.793800000000005</v>
+        <v>62.244500000000002</v>
       </c>
       <c r="E4">
-        <v>96.824700000000007</v>
+        <v>84.124200000000002</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -2348,16 +2348,16 @@
         <v>1978</v>
       </c>
       <c r="B5">
-        <v>104.245</v>
+        <v>89.991900000000001</v>
       </c>
       <c r="C5">
-        <v>7.7301900000000003</v>
+        <v>6.3976800000000003</v>
       </c>
       <c r="D5">
-        <v>89.894599999999997</v>
+        <v>78.078599999999994</v>
       </c>
       <c r="E5">
-        <v>120.886</v>
+        <v>103.723</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2365,16 +2365,16 @@
         <v>1979</v>
       </c>
       <c r="B6">
-        <v>127.91200000000001</v>
+        <v>109.605</v>
       </c>
       <c r="C6">
-        <v>8.5678900000000002</v>
+        <v>7.51288</v>
       </c>
       <c r="D6">
-        <v>111.89100000000001</v>
+        <v>95.578900000000004</v>
       </c>
       <c r="E6">
-        <v>146.227</v>
+        <v>125.68899999999999</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -2382,16 +2382,16 @@
         <v>1980</v>
       </c>
       <c r="B7">
-        <v>141.31399999999999</v>
+        <v>123.764</v>
       </c>
       <c r="C7">
-        <v>9.0793400000000002</v>
+        <v>8.2489500000000007</v>
       </c>
       <c r="D7">
-        <v>124.29</v>
+        <v>108.334</v>
       </c>
       <c r="E7">
-        <v>160.66999999999999</v>
+        <v>141.39099999999999</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -2399,16 +2399,16 @@
         <v>1981</v>
       </c>
       <c r="B8">
-        <v>145.40199999999999</v>
+        <v>128.96299999999999</v>
       </c>
       <c r="C8">
-        <v>9.0981400000000008</v>
+        <v>8.4502600000000001</v>
       </c>
       <c r="D8">
-        <v>128.31399999999999</v>
+        <v>113.139</v>
       </c>
       <c r="E8">
-        <v>164.76599999999999</v>
+        <v>147</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -2416,16 +2416,16 @@
         <v>1982</v>
       </c>
       <c r="B9">
-        <v>140.05600000000001</v>
+        <v>124.673</v>
       </c>
       <c r="C9">
-        <v>8.5926299999999998</v>
+        <v>8.0148799999999998</v>
       </c>
       <c r="D9">
-        <v>123.89700000000001</v>
+        <v>109.646</v>
       </c>
       <c r="E9">
-        <v>158.322</v>
+        <v>141.76</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -2433,16 +2433,16 @@
         <v>1983</v>
       </c>
       <c r="B10">
-        <v>143.18899999999999</v>
+        <v>128.62799999999999</v>
       </c>
       <c r="C10">
-        <v>8.3582800000000006</v>
+        <v>7.8412800000000002</v>
       </c>
       <c r="D10">
-        <v>127.42400000000001</v>
+        <v>113.877</v>
       </c>
       <c r="E10">
-        <v>160.905</v>
+        <v>145.29</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -2450,16 +2450,16 @@
         <v>1984</v>
       </c>
       <c r="B11">
-        <v>158.851</v>
+        <v>144.32900000000001</v>
       </c>
       <c r="C11">
-        <v>8.8728899999999999</v>
+        <v>8.3729700000000005</v>
       </c>
       <c r="D11">
-        <v>142.07300000000001</v>
+        <v>128.53100000000001</v>
       </c>
       <c r="E11">
-        <v>177.61</v>
+        <v>162.06899999999999</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -2467,16 +2467,16 @@
         <v>1985</v>
       </c>
       <c r="B12">
-        <v>156.559</v>
+        <v>142.416</v>
       </c>
       <c r="C12">
-        <v>8.7341800000000003</v>
+        <v>8.1162700000000001</v>
       </c>
       <c r="D12">
-        <v>140.042</v>
+        <v>127.086</v>
       </c>
       <c r="E12">
-        <v>175.024</v>
+        <v>159.595</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -2484,16 +2484,16 @@
         <v>1986</v>
       </c>
       <c r="B13">
-        <v>159.91800000000001</v>
+        <v>148.31899999999999</v>
       </c>
       <c r="C13">
-        <v>8.3685399999999994</v>
+        <v>7.8287899999999997</v>
       </c>
       <c r="D13">
-        <v>144.03700000000001</v>
+        <v>133.46899999999999</v>
       </c>
       <c r="E13">
-        <v>177.54900000000001</v>
+        <v>164.821</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -2501,16 +2501,16 @@
         <v>1987</v>
       </c>
       <c r="B14">
-        <v>183.79300000000001</v>
+        <v>173.923</v>
       </c>
       <c r="C14">
-        <v>9.0130599999999994</v>
+        <v>8.5129199999999994</v>
       </c>
       <c r="D14">
-        <v>166.63300000000001</v>
+        <v>157.71299999999999</v>
       </c>
       <c r="E14">
-        <v>202.721</v>
+        <v>191.79900000000001</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -2518,16 +2518,16 @@
         <v>1988</v>
       </c>
       <c r="B15">
-        <v>185.55600000000001</v>
+        <v>178.01900000000001</v>
       </c>
       <c r="C15">
-        <v>9.0762400000000003</v>
+        <v>8.6409400000000005</v>
       </c>
       <c r="D15">
-        <v>168.273</v>
+        <v>161.55799999999999</v>
       </c>
       <c r="E15">
-        <v>204.614</v>
+        <v>196.15600000000001</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -2535,16 +2535,16 @@
         <v>1989</v>
       </c>
       <c r="B16">
-        <v>188.84399999999999</v>
+        <v>182.81299999999999</v>
       </c>
       <c r="C16">
-        <v>9.9514200000000006</v>
+        <v>9.5342900000000004</v>
       </c>
       <c r="D16">
-        <v>169.96700000000001</v>
+        <v>164.71700000000001</v>
       </c>
       <c r="E16">
-        <v>209.81800000000001</v>
+        <v>202.89699999999999</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -2552,16 +2552,16 @@
         <v>1990</v>
       </c>
       <c r="B17">
-        <v>200.15199999999999</v>
+        <v>195.036</v>
       </c>
       <c r="C17">
-        <v>10.98</v>
+        <v>10.600099999999999</v>
       </c>
       <c r="D17">
-        <v>179.36799999999999</v>
+        <v>174.96199999999999</v>
       </c>
       <c r="E17">
-        <v>223.34299999999999</v>
+        <v>217.41399999999999</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2569,16 +2569,16 @@
         <v>1991</v>
       </c>
       <c r="B18">
-        <v>222.31800000000001</v>
+        <v>217.44900000000001</v>
       </c>
       <c r="C18">
-        <v>11.591100000000001</v>
+        <v>11.232200000000001</v>
       </c>
       <c r="D18">
-        <v>200.31800000000001</v>
+        <v>196.12</v>
       </c>
       <c r="E18">
-        <v>246.73500000000001</v>
+        <v>241.09899999999999</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -2586,16 +2586,16 @@
         <v>1992</v>
       </c>
       <c r="B19">
-        <v>243.13300000000001</v>
+        <v>237.911</v>
       </c>
       <c r="C19">
-        <v>11.9735</v>
+        <v>11.606999999999999</v>
       </c>
       <c r="D19">
-        <v>220.34</v>
+        <v>215.80600000000001</v>
       </c>
       <c r="E19">
-        <v>268.28199999999998</v>
+        <v>262.27999999999997</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -2603,16 +2603,16 @@
         <v>1993</v>
       </c>
       <c r="B20">
-        <v>311.87900000000002</v>
+        <v>304.90199999999999</v>
       </c>
       <c r="C20">
-        <v>14.238300000000001</v>
+        <v>13.801299999999999</v>
       </c>
       <c r="D20">
-        <v>284.678</v>
+        <v>278.52499999999998</v>
       </c>
       <c r="E20">
-        <v>341.68</v>
+        <v>333.77699999999999</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -2620,16 +2620,16 @@
         <v>1994</v>
       </c>
       <c r="B21">
-        <v>369.35399999999998</v>
+        <v>359.827</v>
       </c>
       <c r="C21">
-        <v>15.601000000000001</v>
+        <v>15.097899999999999</v>
       </c>
       <c r="D21">
-        <v>339.447</v>
+        <v>330.875</v>
       </c>
       <c r="E21">
-        <v>401.89699999999999</v>
+        <v>391.31099999999998</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -2637,16 +2637,16 @@
         <v>1995</v>
       </c>
       <c r="B22">
-        <v>433.03800000000001</v>
+        <v>420.24700000000001</v>
       </c>
       <c r="C22">
-        <v>17.411300000000001</v>
+        <v>16.833100000000002</v>
       </c>
       <c r="D22">
-        <v>399.59199999999998</v>
+        <v>387.90600000000001</v>
       </c>
       <c r="E22">
-        <v>469.28399999999999</v>
+        <v>455.28399999999999</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -2654,16 +2654,16 @@
         <v>1996</v>
       </c>
       <c r="B23">
-        <v>547.923</v>
+        <v>529.62199999999996</v>
       </c>
       <c r="C23">
-        <v>22.119399999999999</v>
+        <v>21.488299999999999</v>
       </c>
       <c r="D23">
-        <v>505.43900000000002</v>
+        <v>488.35899999999998</v>
       </c>
       <c r="E23">
-        <v>593.97699999999998</v>
+        <v>574.37199999999996</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -2671,16 +2671,16 @@
         <v>1997</v>
       </c>
       <c r="B24">
-        <v>601.32000000000005</v>
+        <v>581.64300000000003</v>
       </c>
       <c r="C24">
-        <v>23.994199999999999</v>
+        <v>23.322800000000001</v>
       </c>
       <c r="D24">
-        <v>555.21400000000006</v>
+        <v>536.83600000000001</v>
       </c>
       <c r="E24">
-        <v>651.25400000000002</v>
+        <v>630.18899999999996</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -2688,16 +2688,16 @@
         <v>1998</v>
       </c>
       <c r="B25">
-        <v>585.53700000000003</v>
+        <v>566.88300000000004</v>
       </c>
       <c r="C25">
-        <v>23.0457</v>
+        <v>22.4133</v>
       </c>
       <c r="D25">
-        <v>541.22900000000004</v>
+        <v>523.79999999999995</v>
       </c>
       <c r="E25">
-        <v>633.471</v>
+        <v>613.51099999999997</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -2705,16 +2705,16 @@
         <v>1999</v>
       </c>
       <c r="B26">
-        <v>611.36</v>
+        <v>593.21699999999998</v>
       </c>
       <c r="C26">
-        <v>23.217300000000002</v>
+        <v>22.642600000000002</v>
       </c>
       <c r="D26">
-        <v>566.66</v>
+        <v>549.63300000000004</v>
       </c>
       <c r="E26">
-        <v>659.58500000000004</v>
+        <v>640.25800000000004</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -2722,16 +2722,16 @@
         <v>2000</v>
       </c>
       <c r="B27">
-        <v>642.36099999999999</v>
+        <v>624.13400000000001</v>
       </c>
       <c r="C27">
-        <v>23.875699999999998</v>
+        <v>23.321400000000001</v>
       </c>
       <c r="D27">
-        <v>596.35699999999997</v>
+        <v>579.20699999999999</v>
       </c>
       <c r="E27">
-        <v>691.91399999999999</v>
+        <v>672.54600000000005</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -2739,16 +2739,16 @@
         <v>2001</v>
       </c>
       <c r="B28">
-        <v>655.26300000000003</v>
+        <v>638.65200000000004</v>
       </c>
       <c r="C28">
-        <v>24.255400000000002</v>
+        <v>23.796099999999999</v>
       </c>
       <c r="D28">
-        <v>608.52</v>
+        <v>592.80499999999995</v>
       </c>
       <c r="E28">
-        <v>705.59699999999998</v>
+        <v>688.04499999999996</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -2756,16 +2756,16 @@
         <v>2002</v>
       </c>
       <c r="B29">
-        <v>658.74599999999998</v>
+        <v>644.01099999999997</v>
       </c>
       <c r="C29">
-        <v>23.820399999999999</v>
+        <v>23.438199999999998</v>
       </c>
       <c r="D29">
-        <v>612.80200000000002</v>
+        <v>598.81399999999996</v>
       </c>
       <c r="E29">
-        <v>708.13499999999999</v>
+        <v>692.61900000000003</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -2773,16 +2773,16 @@
         <v>2003</v>
       </c>
       <c r="B30">
-        <v>663.41399999999999</v>
+        <v>650.9</v>
       </c>
       <c r="C30">
-        <v>23.872199999999999</v>
+        <v>23.584099999999999</v>
       </c>
       <c r="D30">
-        <v>617.36199999999997</v>
+        <v>605.41399999999999</v>
       </c>
       <c r="E30">
-        <v>712.90200000000004</v>
+        <v>699.80200000000002</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -2790,16 +2790,16 @@
         <v>2004</v>
       </c>
       <c r="B31">
-        <v>645.76499999999999</v>
+        <v>634.87800000000004</v>
       </c>
       <c r="C31">
-        <v>23.114100000000001</v>
+        <v>22.869599999999998</v>
       </c>
       <c r="D31">
-        <v>601.16700000000003</v>
+        <v>590.76099999999997</v>
       </c>
       <c r="E31">
-        <v>693.67200000000003</v>
+        <v>682.28899999999999</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -2807,16 +2807,16 @@
         <v>2005</v>
       </c>
       <c r="B32">
-        <v>538.55399999999997</v>
+        <v>531.99099999999999</v>
       </c>
       <c r="C32">
-        <v>19.578199999999999</v>
+        <v>19.477900000000002</v>
       </c>
       <c r="D32">
-        <v>500.79899999999998</v>
+        <v>494.43900000000002</v>
       </c>
       <c r="E32">
-        <v>579.15499999999997</v>
+        <v>572.39400000000001</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -2824,16 +2824,16 @@
         <v>2006</v>
       </c>
       <c r="B33">
-        <v>483.59500000000003</v>
+        <v>480.23200000000003</v>
       </c>
       <c r="C33">
-        <v>17.755199999999999</v>
+        <v>17.765899999999998</v>
       </c>
       <c r="D33">
-        <v>449.36799999999999</v>
+        <v>445.99400000000003</v>
       </c>
       <c r="E33">
-        <v>520.42899999999997</v>
+        <v>517.09799999999996</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -2841,16 +2841,16 @@
         <v>2007</v>
       </c>
       <c r="B34">
-        <v>455.548</v>
+        <v>453.416</v>
       </c>
       <c r="C34">
-        <v>16.848500000000001</v>
+        <v>16.898199999999999</v>
       </c>
       <c r="D34">
-        <v>423.07799999999997</v>
+        <v>420.85899999999998</v>
       </c>
       <c r="E34">
-        <v>490.51100000000002</v>
+        <v>488.49099999999999</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -2858,16 +2858,16 @@
         <v>2008</v>
       </c>
       <c r="B35">
-        <v>443.50599999999997</v>
+        <v>440.98700000000002</v>
       </c>
       <c r="C35">
-        <v>16.354299999999999</v>
+        <v>16.387499999999999</v>
       </c>
       <c r="D35">
-        <v>411.98500000000001</v>
+        <v>409.411</v>
       </c>
       <c r="E35">
-        <v>477.43900000000002</v>
+        <v>474.99900000000002</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -2875,16 +2875,16 @@
         <v>2009</v>
       </c>
       <c r="B36">
-        <v>402.286</v>
+        <v>399.97699999999998</v>
       </c>
       <c r="C36">
-        <v>15.084199999999999</v>
+        <v>15.1449</v>
       </c>
       <c r="D36">
-        <v>373.23099999999999</v>
+        <v>370.815</v>
       </c>
       <c r="E36">
-        <v>433.60300000000001</v>
+        <v>431.43099999999998</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -2892,16 +2892,16 @@
         <v>2010</v>
       </c>
       <c r="B37">
-        <v>439.35899999999998</v>
+        <v>434.41300000000001</v>
       </c>
       <c r="C37">
-        <v>16.438199999999998</v>
+        <v>16.399899999999999</v>
       </c>
       <c r="D37">
-        <v>407.69400000000002</v>
+        <v>402.83199999999999</v>
       </c>
       <c r="E37">
-        <v>473.48500000000001</v>
+        <v>468.471</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -2909,16 +2909,16 @@
         <v>2011</v>
       </c>
       <c r="B38">
-        <v>516.38499999999999</v>
+        <v>507.52499999999998</v>
       </c>
       <c r="C38">
-        <v>19.364100000000001</v>
+        <v>19.160699999999999</v>
       </c>
       <c r="D38">
-        <v>479.08600000000001</v>
+        <v>470.62799999999999</v>
       </c>
       <c r="E38">
-        <v>556.58799999999997</v>
+        <v>547.31600000000003</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -2926,16 +2926,16 @@
         <v>2012</v>
       </c>
       <c r="B39">
-        <v>568.06100000000004</v>
+        <v>556.77499999999998</v>
       </c>
       <c r="C39">
-        <v>21.761800000000001</v>
+        <v>21.450299999999999</v>
       </c>
       <c r="D39">
-        <v>526.178</v>
+        <v>515.5</v>
       </c>
       <c r="E39">
-        <v>613.27800000000002</v>
+        <v>601.35400000000004</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -2943,16 +2943,16 @@
         <v>2013</v>
       </c>
       <c r="B40">
-        <v>593.66</v>
+        <v>580.71799999999996</v>
       </c>
       <c r="C40">
-        <v>23.567399999999999</v>
+        <v>23.182500000000001</v>
       </c>
       <c r="D40">
-        <v>548.36500000000001</v>
+        <v>536.173</v>
       </c>
       <c r="E40">
-        <v>642.69600000000003</v>
+        <v>628.96400000000006</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -2960,16 +2960,16 @@
         <v>2014</v>
       </c>
       <c r="B41">
-        <v>608.99599999999998</v>
+        <v>596.29999999999995</v>
       </c>
       <c r="C41">
-        <v>24.632300000000001</v>
+        <v>24.255800000000001</v>
       </c>
       <c r="D41">
-        <v>561.69000000000005</v>
+        <v>549.72799999999995</v>
       </c>
       <c r="E41">
-        <v>660.28599999999994</v>
+        <v>646.81799999999998</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -2977,16 +2977,16 @@
         <v>2015</v>
       </c>
       <c r="B42">
-        <v>631.53300000000002</v>
+        <v>619.71500000000003</v>
       </c>
       <c r="C42">
-        <v>25.9651</v>
+        <v>25.619499999999999</v>
       </c>
       <c r="D42">
-        <v>581.70100000000002</v>
+        <v>570.55700000000002</v>
       </c>
       <c r="E42">
-        <v>685.63400000000001</v>
+        <v>673.10799999999995</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -2994,16 +2994,16 @@
         <v>2016</v>
       </c>
       <c r="B43">
-        <v>556.82899999999995</v>
+        <v>549.38599999999997</v>
       </c>
       <c r="C43">
-        <v>23.373200000000001</v>
+        <v>23.209599999999998</v>
       </c>
       <c r="D43">
-        <v>512.01</v>
+        <v>504.892</v>
       </c>
       <c r="E43">
-        <v>605.572</v>
+        <v>597.79999999999995</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3011,16 +3011,16 @@
         <v>2017</v>
       </c>
       <c r="B44">
-        <v>491.26499999999999</v>
+        <v>487.75799999999998</v>
       </c>
       <c r="C44">
-        <v>21.3765</v>
+        <v>21.374400000000001</v>
       </c>
       <c r="D44">
-        <v>450.33800000000002</v>
+        <v>446.84800000000001</v>
       </c>
       <c r="E44">
-        <v>535.91200000000003</v>
+        <v>532.41399999999999</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3028,16 +3028,16 @@
         <v>2018</v>
       </c>
       <c r="B45">
-        <v>415.68200000000002</v>
+        <v>415.495</v>
       </c>
       <c r="C45">
-        <v>18.7577</v>
+        <v>18.877500000000001</v>
       </c>
       <c r="D45">
-        <v>379.827</v>
+        <v>379.423</v>
       </c>
       <c r="E45">
-        <v>454.92200000000003</v>
+        <v>454.99799999999999</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3045,16 +3045,16 @@
         <v>2019</v>
       </c>
       <c r="B46">
-        <v>363.65100000000001</v>
+        <v>365.93900000000002</v>
       </c>
       <c r="C46">
-        <v>17.005099999999999</v>
+        <v>17.206099999999999</v>
       </c>
       <c r="D46">
-        <v>331.2</v>
+        <v>333.11200000000002</v>
       </c>
       <c r="E46">
-        <v>399.28199999999998</v>
+        <v>402</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3062,16 +3062,16 @@
         <v>2020</v>
       </c>
       <c r="B47">
-        <v>313.97699999999998</v>
+        <v>318.46199999999999</v>
       </c>
       <c r="C47">
-        <v>15.3104</v>
+        <v>15.5929</v>
       </c>
       <c r="D47">
-        <v>284.81900000000002</v>
+        <v>288.77100000000002</v>
       </c>
       <c r="E47">
-        <v>346.12099999999998</v>
+        <v>351.20499999999998</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3079,16 +3079,16 @@
         <v>2021</v>
       </c>
       <c r="B48">
-        <v>271.46899999999999</v>
+        <v>277.30399999999997</v>
       </c>
       <c r="C48">
-        <v>13.734400000000001</v>
+        <v>14.063599999999999</v>
       </c>
       <c r="D48">
-        <v>245.36</v>
+        <v>250.57300000000001</v>
       </c>
       <c r="E48">
-        <v>300.35599999999999</v>
+        <v>306.887</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3096,16 +3096,16 @@
         <v>2022</v>
       </c>
       <c r="B49">
-        <v>254.077</v>
+        <v>260.44099999999997</v>
       </c>
       <c r="C49">
-        <v>12.8376</v>
+        <v>13.1814</v>
       </c>
       <c r="D49">
-        <v>229.672</v>
+        <v>235.38399999999999</v>
       </c>
       <c r="E49">
-        <v>281.077</v>
+        <v>288.166</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3113,16 +3113,16 @@
         <v>2023</v>
       </c>
       <c r="B50">
-        <v>247.87299999999999</v>
+        <v>254.16</v>
       </c>
       <c r="C50">
-        <v>12.358499999999999</v>
+        <v>12.6996</v>
       </c>
       <c r="D50">
-        <v>224.36199999999999</v>
+        <v>230.00299999999999</v>
       </c>
       <c r="E50">
-        <v>273.84800000000001</v>
+        <v>280.85399999999998</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -3130,16 +3130,16 @@
         <v>2024</v>
       </c>
       <c r="B51">
-        <v>266.26400000000001</v>
+        <v>271.988</v>
       </c>
       <c r="C51">
-        <v>13.367100000000001</v>
+        <v>13.6686</v>
       </c>
       <c r="D51">
-        <v>240.84299999999999</v>
+        <v>245.99600000000001</v>
       </c>
       <c r="E51">
-        <v>294.36700000000002</v>
+        <v>300.72800000000001</v>
       </c>
     </row>
   </sheetData>
@@ -3152,7 +3152,7 @@
   <dimension ref="A1:E51"/>
   <sheetViews>
     <sheetView topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B51"/>
+      <selection activeCell="B2" sqref="B2:B51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -3179,16 +3179,16 @@
         <v>1975</v>
       </c>
       <c r="B2">
-        <v>290.47300000000001</v>
+        <v>246.19300000000001</v>
       </c>
       <c r="C2">
-        <v>19.590800000000002</v>
+        <v>14.9946</v>
       </c>
       <c r="D2">
-        <v>253.858</v>
+        <v>217.983</v>
       </c>
       <c r="E2">
-        <v>332.36900000000003</v>
+        <v>278.05399999999997</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -3196,16 +3196,16 @@
         <v>1976</v>
       </c>
       <c r="B3">
-        <v>320.43799999999999</v>
+        <v>266.55599999999998</v>
       </c>
       <c r="C3">
-        <v>21.2057</v>
+        <v>16.382200000000001</v>
       </c>
       <c r="D3">
-        <v>280.75400000000002</v>
+        <v>235.75200000000001</v>
       </c>
       <c r="E3">
-        <v>365.73099999999999</v>
+        <v>301.38400000000001</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -3213,16 +3213,16 @@
         <v>1977</v>
       </c>
       <c r="B4">
-        <v>343.23099999999999</v>
+        <v>283.40300000000002</v>
       </c>
       <c r="C4">
-        <v>21.977599999999999</v>
+        <v>17.1921</v>
       </c>
       <c r="D4">
-        <v>302.01400000000001</v>
+        <v>251.05099999999999</v>
       </c>
       <c r="E4">
-        <v>390.07400000000001</v>
+        <v>319.92399999999998</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -3230,16 +3230,16 @@
         <v>1978</v>
       </c>
       <c r="B5">
-        <v>366.041</v>
+        <v>304.36599999999999</v>
       </c>
       <c r="C5">
-        <v>22.2166</v>
+        <v>17.6021</v>
       </c>
       <c r="D5">
-        <v>324.23500000000001</v>
+        <v>271.14800000000002</v>
       </c>
       <c r="E5">
-        <v>413.23700000000002</v>
+        <v>341.654</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -3247,16 +3247,16 @@
         <v>1979</v>
       </c>
       <c r="B6">
-        <v>382.20400000000001</v>
+        <v>322.49299999999999</v>
       </c>
       <c r="C6">
-        <v>21.946200000000001</v>
+        <v>17.615300000000001</v>
       </c>
       <c r="D6">
-        <v>340.77</v>
+        <v>289.142</v>
       </c>
       <c r="E6">
-        <v>428.67500000000001</v>
+        <v>359.69099999999997</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
@@ -3264,16 +3264,16 @@
         <v>1980</v>
       </c>
       <c r="B7">
-        <v>405.12599999999998</v>
+        <v>348.09899999999999</v>
       </c>
       <c r="C7">
-        <v>21.650600000000001</v>
+        <v>17.638000000000002</v>
       </c>
       <c r="D7">
-        <v>364.08600000000001</v>
+        <v>314.572</v>
       </c>
       <c r="E7">
-        <v>450.791</v>
+        <v>385.19900000000001</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
@@ -3281,16 +3281,16 @@
         <v>1981</v>
       </c>
       <c r="B8">
-        <v>470.68099999999998</v>
+        <v>414.471</v>
       </c>
       <c r="C8">
-        <v>22.953700000000001</v>
+        <v>19.047899999999998</v>
       </c>
       <c r="D8">
-        <v>426.96600000000001</v>
+        <v>378.09199999999998</v>
       </c>
       <c r="E8">
-        <v>518.87099999999998</v>
+        <v>454.351</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
@@ -3298,16 +3298,16 @@
         <v>1982</v>
       </c>
       <c r="B9">
-        <v>494.00400000000002</v>
+        <v>442.64400000000001</v>
       </c>
       <c r="C9">
-        <v>22.42</v>
+        <v>18.932700000000001</v>
       </c>
       <c r="D9">
-        <v>451.15899999999999</v>
+        <v>406.36900000000003</v>
       </c>
       <c r="E9">
-        <v>540.91600000000005</v>
+        <v>482.15800000000002</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
@@ -3315,16 +3315,16 @@
         <v>1983</v>
       </c>
       <c r="B10">
-        <v>575.19500000000005</v>
+        <v>525.47</v>
       </c>
       <c r="C10">
-        <v>24.534300000000002</v>
+        <v>21.2819</v>
       </c>
       <c r="D10">
-        <v>528.18200000000002</v>
+        <v>484.601</v>
       </c>
       <c r="E10">
-        <v>626.39400000000001</v>
+        <v>569.78700000000003</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
@@ -3332,16 +3332,16 @@
         <v>1984</v>
       </c>
       <c r="B11">
-        <v>618.46299999999997</v>
+        <v>571.47500000000002</v>
       </c>
       <c r="C11">
-        <v>25.198</v>
+        <v>22.183599999999998</v>
       </c>
       <c r="D11">
-        <v>570.08500000000004</v>
+        <v>528.80200000000002</v>
       </c>
       <c r="E11">
-        <v>670.94600000000003</v>
+        <v>617.59199999999998</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
@@ -3349,16 +3349,16 @@
         <v>1985</v>
       </c>
       <c r="B12">
-        <v>803.61599999999999</v>
+        <v>748.97799999999995</v>
       </c>
       <c r="C12">
-        <v>32.2029</v>
+        <v>28.723199999999999</v>
       </c>
       <c r="D12">
-        <v>741.74800000000005</v>
+        <v>693.69899999999996</v>
       </c>
       <c r="E12">
-        <v>870.64499999999998</v>
+        <v>808.66200000000003</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
@@ -3366,16 +3366,16 @@
         <v>1986</v>
       </c>
       <c r="B13">
-        <v>790.01800000000003</v>
+        <v>739.54300000000001</v>
       </c>
       <c r="C13">
-        <v>30.6799</v>
+        <v>27.546099999999999</v>
       </c>
       <c r="D13">
-        <v>731.00199999999995</v>
+        <v>686.471</v>
       </c>
       <c r="E13">
-        <v>853.79899999999998</v>
+        <v>796.71900000000005</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
@@ -3383,16 +3383,16 @@
         <v>1987</v>
       </c>
       <c r="B14">
-        <v>1038.33</v>
+        <v>979.56</v>
       </c>
       <c r="C14">
-        <v>39.1449</v>
+        <v>35.512900000000002</v>
       </c>
       <c r="D14">
-        <v>962.94600000000003</v>
+        <v>911.07</v>
       </c>
       <c r="E14">
-        <v>1119.6199999999999</v>
+        <v>1053.2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
@@ -3400,16 +3400,16 @@
         <v>1988</v>
       </c>
       <c r="B15">
-        <v>1155.5899999999999</v>
+        <v>1089.56</v>
       </c>
       <c r="C15">
-        <v>44.005000000000003</v>
+        <v>39.999099999999999</v>
       </c>
       <c r="D15">
-        <v>1070.8699999999999</v>
+        <v>1012.45</v>
       </c>
       <c r="E15">
-        <v>1247</v>
+        <v>1172.54</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -3417,16 +3417,16 @@
         <v>1989</v>
       </c>
       <c r="B16">
-        <v>1207.74</v>
+        <v>1133.4100000000001</v>
       </c>
       <c r="C16">
-        <v>48.4953</v>
+        <v>44.081400000000002</v>
       </c>
       <c r="D16">
-        <v>1114.58</v>
+        <v>1048.6199999999999</v>
       </c>
       <c r="E16">
-        <v>1308.69</v>
+        <v>1225.05</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -3434,16 +3434,16 @@
         <v>1990</v>
       </c>
       <c r="B17">
-        <v>1153.3800000000001</v>
+        <v>1084.7</v>
       </c>
       <c r="C17">
-        <v>46.845999999999997</v>
+        <v>42.865000000000002</v>
       </c>
       <c r="D17">
-        <v>1063.43</v>
+        <v>1002.3</v>
       </c>
       <c r="E17">
-        <v>1250.94</v>
+        <v>1173.8699999999999</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -3451,16 +3451,16 @@
         <v>1991</v>
       </c>
       <c r="B18">
-        <v>1250.74</v>
+        <v>1173.1300000000001</v>
       </c>
       <c r="C18">
-        <v>50.8932</v>
+        <v>46.5289</v>
       </c>
       <c r="D18">
-        <v>1153.03</v>
+        <v>1083.7</v>
       </c>
       <c r="E18">
-        <v>1356.74</v>
+        <v>1269.94</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
@@ -3468,16 +3468,16 @@
         <v>1992</v>
       </c>
       <c r="B19">
-        <v>1281.95</v>
+        <v>1201.06</v>
       </c>
       <c r="C19">
-        <v>52.459200000000003</v>
+        <v>48.044600000000003</v>
       </c>
       <c r="D19">
-        <v>1181.25</v>
+        <v>1108.75</v>
       </c>
       <c r="E19">
-        <v>1391.24</v>
+        <v>1301.05</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
@@ -3485,16 +3485,16 @@
         <v>1993</v>
       </c>
       <c r="B20">
-        <v>1562.74</v>
+        <v>1463.42</v>
       </c>
       <c r="C20">
-        <v>64.179299999999998</v>
+        <v>58.929099999999998</v>
       </c>
       <c r="D20">
-        <v>1439.56</v>
+        <v>1350.23</v>
       </c>
       <c r="E20">
-        <v>1696.45</v>
+        <v>1586.1</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
@@ -3502,16 +3502,16 @@
         <v>1994</v>
       </c>
       <c r="B21">
-        <v>1702.29</v>
+        <v>1593.47</v>
       </c>
       <c r="C21">
-        <v>70.132199999999997</v>
+        <v>64.559600000000003</v>
       </c>
       <c r="D21">
-        <v>1567.71</v>
+        <v>1469.5</v>
       </c>
       <c r="E21">
-        <v>1848.44</v>
+        <v>1727.91</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -3519,16 +3519,16 @@
         <v>1995</v>
       </c>
       <c r="B22">
-        <v>1711.42</v>
+        <v>1604.55</v>
       </c>
       <c r="C22">
-        <v>69.943700000000007</v>
+        <v>64.662999999999997</v>
       </c>
       <c r="D22">
-        <v>1577.15</v>
+        <v>1480.35</v>
       </c>
       <c r="E22">
-        <v>1857.12</v>
+        <v>1739.18</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -3536,16 +3536,16 @@
         <v>1996</v>
       </c>
       <c r="B23">
-        <v>1820.56</v>
+        <v>1710.33</v>
       </c>
       <c r="C23">
-        <v>73.212800000000001</v>
+        <v>67.974999999999994</v>
       </c>
       <c r="D23">
-        <v>1679.92</v>
+        <v>1579.7</v>
       </c>
       <c r="E23">
-        <v>1972.97</v>
+        <v>1851.77</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -3553,16 +3553,16 @@
         <v>1997</v>
       </c>
       <c r="B24">
-        <v>1741.27</v>
+        <v>1641.42</v>
       </c>
       <c r="C24">
-        <v>68.199100000000001</v>
+        <v>63.627400000000002</v>
       </c>
       <c r="D24">
-        <v>1610.13</v>
+        <v>1519.02</v>
       </c>
       <c r="E24">
-        <v>1883.1</v>
+        <v>1773.69</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -3570,16 +3570,16 @@
         <v>1998</v>
       </c>
       <c r="B25">
-        <v>1585.61</v>
+        <v>1498.86</v>
       </c>
       <c r="C25">
-        <v>61.093299999999999</v>
+        <v>57.2712</v>
       </c>
       <c r="D25">
-        <v>1468.06</v>
+        <v>1388.63</v>
       </c>
       <c r="E25">
-        <v>1712.58</v>
+        <v>1617.85</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -3587,16 +3587,16 @@
         <v>1999</v>
       </c>
       <c r="B26">
-        <v>1400.1</v>
+        <v>1331.37</v>
       </c>
       <c r="C26">
-        <v>51.899299999999997</v>
+        <v>49.052399999999999</v>
       </c>
       <c r="D26">
-        <v>1300.0899999999999</v>
+        <v>1236.82</v>
       </c>
       <c r="E26">
-        <v>1507.81</v>
+        <v>1433.15</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
@@ -3604,16 +3604,16 @@
         <v>2000</v>
       </c>
       <c r="B27">
-        <v>1356.95</v>
+        <v>1294.8399999999999</v>
       </c>
       <c r="C27">
-        <v>49.274900000000002</v>
+        <v>46.8123</v>
       </c>
       <c r="D27">
-        <v>1261.93</v>
+        <v>1204.55</v>
       </c>
       <c r="E27">
-        <v>1459.13</v>
+        <v>1391.9</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
@@ -3621,16 +3621,16 @@
         <v>2001</v>
       </c>
       <c r="B28">
-        <v>1431.4</v>
+        <v>1367.23</v>
       </c>
       <c r="C28">
-        <v>51.7622</v>
+        <v>49.254399999999997</v>
       </c>
       <c r="D28">
-        <v>1331.56</v>
+        <v>1272.21</v>
       </c>
       <c r="E28">
-        <v>1538.72</v>
+        <v>1469.34</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -3638,16 +3638,16 @@
         <v>2002</v>
       </c>
       <c r="B29">
-        <v>1427.23</v>
+        <v>1365.73</v>
       </c>
       <c r="C29">
-        <v>50.615200000000002</v>
+        <v>48.222000000000001</v>
       </c>
       <c r="D29">
-        <v>1329.54</v>
+        <v>1272.6400000000001</v>
       </c>
       <c r="E29">
-        <v>1532.1</v>
+        <v>1465.63</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -3655,16 +3655,16 @@
         <v>2003</v>
       </c>
       <c r="B30">
-        <v>1481.92</v>
+        <v>1418.69</v>
       </c>
       <c r="C30">
-        <v>52.314700000000002</v>
+        <v>49.830399999999997</v>
       </c>
       <c r="D30">
-        <v>1380.93</v>
+        <v>1322.47</v>
       </c>
       <c r="E30">
-        <v>1590.3</v>
+        <v>1521.9</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
@@ -3672,16 +3672,16 @@
         <v>2004</v>
       </c>
       <c r="B31">
-        <v>1761.77</v>
+        <v>1675.15</v>
       </c>
       <c r="C31">
-        <v>64.412899999999993</v>
+        <v>60.567799999999998</v>
       </c>
       <c r="D31">
-        <v>1637.58</v>
+        <v>1558.32</v>
       </c>
       <c r="E31">
-        <v>1895.37</v>
+        <v>1800.73</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
@@ -3689,16 +3689,16 @@
         <v>2005</v>
       </c>
       <c r="B32">
-        <v>1576.9</v>
+        <v>1500.9</v>
       </c>
       <c r="C32">
-        <v>57.545499999999997</v>
+        <v>54.153500000000001</v>
       </c>
       <c r="D32">
-        <v>1465.94</v>
+        <v>1396.44</v>
       </c>
       <c r="E32">
-        <v>1696.25</v>
+        <v>1613.17</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
@@ -3706,16 +3706,16 @@
         <v>2006</v>
       </c>
       <c r="B33">
-        <v>1433.05</v>
+        <v>1366.94</v>
       </c>
       <c r="C33">
-        <v>51.690300000000001</v>
+        <v>48.752099999999999</v>
       </c>
       <c r="D33">
-        <v>1333.34</v>
+        <v>1272.8599999999999</v>
       </c>
       <c r="E33">
-        <v>1540.21</v>
+        <v>1467.97</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
@@ -3723,16 +3723,16 @@
         <v>2007</v>
       </c>
       <c r="B34">
-        <v>1418.96</v>
+        <v>1354.31</v>
       </c>
       <c r="C34">
-        <v>51.162300000000002</v>
+        <v>48.256399999999999</v>
       </c>
       <c r="D34">
-        <v>1320.27</v>
+        <v>1261.18</v>
       </c>
       <c r="E34">
-        <v>1525.03</v>
+        <v>1454.31</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -3740,16 +3740,16 @@
         <v>2008</v>
       </c>
       <c r="B35">
-        <v>1468</v>
+        <v>1400.55</v>
       </c>
       <c r="C35">
-        <v>53.350900000000003</v>
+        <v>50.258499999999998</v>
       </c>
       <c r="D35">
-        <v>1365.12</v>
+        <v>1303.58</v>
       </c>
       <c r="E35">
-        <v>1578.64</v>
+        <v>1504.72</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
@@ -3757,16 +3757,16 @@
         <v>2009</v>
       </c>
       <c r="B36">
-        <v>1393.44</v>
+        <v>1330.13</v>
       </c>
       <c r="C36">
-        <v>51.207000000000001</v>
+        <v>48.287500000000001</v>
       </c>
       <c r="D36">
-        <v>1294.74</v>
+        <v>1237.01</v>
       </c>
       <c r="E36">
-        <v>1499.68</v>
+        <v>1430.26</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
@@ -3774,16 +3774,16 @@
         <v>2010</v>
       </c>
       <c r="B37">
-        <v>1468.27</v>
+        <v>1401.7</v>
       </c>
       <c r="C37">
-        <v>54.741399999999999</v>
+        <v>51.648200000000003</v>
       </c>
       <c r="D37">
-        <v>1362.8</v>
+        <v>1302.1500000000001</v>
       </c>
       <c r="E37">
-        <v>1581.89</v>
+        <v>1508.86</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -3791,16 +3791,16 @@
         <v>2011</v>
       </c>
       <c r="B38">
-        <v>1661.8</v>
+        <v>1586.57</v>
       </c>
       <c r="C38">
-        <v>63.217500000000001</v>
+        <v>59.6828</v>
       </c>
       <c r="D38">
-        <v>1540.1</v>
+        <v>1471.63</v>
       </c>
       <c r="E38">
-        <v>1793.12</v>
+        <v>1710.5</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -3808,16 +3808,16 @@
         <v>2012</v>
       </c>
       <c r="B39">
-        <v>1504.86</v>
+        <v>1443.27</v>
       </c>
       <c r="C39">
-        <v>56.9191</v>
+        <v>54.155000000000001</v>
       </c>
       <c r="D39">
-        <v>1395.26</v>
+        <v>1338.96</v>
       </c>
       <c r="E39">
-        <v>1623.07</v>
+        <v>1555.7</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
@@ -3825,16 +3825,16 @@
         <v>2013</v>
       </c>
       <c r="B40">
-        <v>1363.23</v>
+        <v>1311.75</v>
       </c>
       <c r="C40">
-        <v>52.6036</v>
+        <v>50.3977</v>
       </c>
       <c r="D40">
-        <v>1262.01</v>
+        <v>1214.76</v>
       </c>
       <c r="E40">
-        <v>1472.56</v>
+        <v>1416.47</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
@@ -3842,16 +3842,16 @@
         <v>2014</v>
       </c>
       <c r="B41">
-        <v>1191.54</v>
+        <v>1152.21</v>
       </c>
       <c r="C41">
-        <v>46.372300000000003</v>
+        <v>44.796500000000002</v>
       </c>
       <c r="D41">
-        <v>1102.3499999999999</v>
+        <v>1066.04</v>
       </c>
       <c r="E41">
-        <v>1287.95</v>
+        <v>1245.3399999999999</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
@@ -3859,16 +3859,16 @@
         <v>2015</v>
       </c>
       <c r="B42">
-        <v>1176.08</v>
+        <v>1141.51</v>
       </c>
       <c r="C42">
-        <v>46.505299999999998</v>
+        <v>45.163400000000003</v>
       </c>
       <c r="D42">
-        <v>1086.69</v>
+        <v>1054.7</v>
       </c>
       <c r="E42">
-        <v>1272.83</v>
+        <v>1235.47</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -3876,16 +3876,16 @@
         <v>2016</v>
       </c>
       <c r="B43">
-        <v>1009.33</v>
+        <v>984.37599999999998</v>
       </c>
       <c r="C43">
-        <v>40.565600000000003</v>
+        <v>39.6584</v>
       </c>
       <c r="D43">
-        <v>931.40300000000002</v>
+        <v>908.2</v>
       </c>
       <c r="E43">
-        <v>1093.77</v>
+        <v>1066.94</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
@@ -3893,16 +3893,16 @@
         <v>2017</v>
       </c>
       <c r="B44">
-        <v>896.64300000000003</v>
+        <v>878.125</v>
       </c>
       <c r="C44">
-        <v>36.817399999999999</v>
+        <v>36.208799999999997</v>
       </c>
       <c r="D44">
-        <v>825.97900000000004</v>
+        <v>808.64200000000005</v>
       </c>
       <c r="E44">
-        <v>973.35199999999998</v>
+        <v>953.57899999999995</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
@@ -3910,16 +3910,16 @@
         <v>2018</v>
       </c>
       <c r="B45">
-        <v>843.89099999999996</v>
+        <v>827.529</v>
       </c>
       <c r="C45">
-        <v>35.304000000000002</v>
+        <v>34.746499999999997</v>
       </c>
       <c r="D45">
-        <v>776.18399999999997</v>
+        <v>760.90200000000004</v>
       </c>
       <c r="E45">
-        <v>917.50300000000004</v>
+        <v>899.99</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
@@ -3927,16 +3927,16 @@
         <v>2019</v>
       </c>
       <c r="B46">
-        <v>879.02800000000002</v>
+        <v>860.53300000000002</v>
       </c>
       <c r="C46">
-        <v>37.5002</v>
+        <v>36.716000000000001</v>
       </c>
       <c r="D46">
-        <v>807.16899999999998</v>
+        <v>790.178</v>
       </c>
       <c r="E46">
-        <v>957.28399999999999</v>
+        <v>937.15300000000002</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
@@ -3944,16 +3944,16 @@
         <v>2020</v>
       </c>
       <c r="B47">
-        <v>908.42399999999998</v>
+        <v>888.68600000000004</v>
       </c>
       <c r="C47">
-        <v>39.736400000000003</v>
+        <v>38.7119</v>
       </c>
       <c r="D47">
-        <v>832.36300000000006</v>
+        <v>814.572</v>
       </c>
       <c r="E47">
-        <v>991.43499999999995</v>
+        <v>969.54200000000003</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
@@ -3961,16 +3961,16 @@
         <v>2021</v>
       </c>
       <c r="B48">
-        <v>940.83799999999997</v>
+        <v>920.86500000000001</v>
       </c>
       <c r="C48">
-        <v>42.963900000000002</v>
+        <v>41.675899999999999</v>
       </c>
       <c r="D48">
-        <v>858.75800000000004</v>
+        <v>841.21299999999997</v>
       </c>
       <c r="E48">
-        <v>1030.76</v>
+        <v>1008.06</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
@@ -3978,16 +3978,16 @@
         <v>2022</v>
       </c>
       <c r="B49">
-        <v>1018.1</v>
+        <v>998.39</v>
       </c>
       <c r="C49">
-        <v>49.923200000000001</v>
+        <v>48.235300000000002</v>
       </c>
       <c r="D49">
-        <v>923.04899999999998</v>
+        <v>906.48500000000001</v>
       </c>
       <c r="E49">
-        <v>1122.94</v>
+        <v>1099.6099999999999</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
@@ -3995,16 +3995,16 @@
         <v>2023</v>
       </c>
       <c r="B50">
-        <v>1033.19</v>
+        <v>1020.84</v>
       </c>
       <c r="C50">
-        <v>55.968800000000002</v>
+        <v>54.510899999999999</v>
       </c>
       <c r="D50">
-        <v>927.17200000000003</v>
+        <v>917.50300000000004</v>
       </c>
       <c r="E50">
-        <v>1151.32</v>
+        <v>1135.81</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
@@ -4012,16 +4012,16 @@
         <v>2024</v>
       </c>
       <c r="B51">
-        <v>1048.79</v>
+        <v>1051.04</v>
       </c>
       <c r="C51">
-        <v>64.652500000000003</v>
+        <v>64.692700000000002</v>
       </c>
       <c r="D51">
-        <v>927.245</v>
+        <v>929.40800000000002</v>
       </c>
       <c r="E51">
-        <v>1186.26</v>
+        <v>1188.5899999999999</v>
       </c>
     </row>
   </sheetData>

</xml_diff>